<commit_message>
Foodics API + Consolidated Invoice + edit in General Journal
</commit_message>
<xml_diff>
--- a/Store Statistics/src/Store Consumption Statistics.xlsx
+++ b/Store Statistics/src/Store Consumption Statistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alsubaihisons-my.sharepoint.com/personal/a_khoriez_alsubaihisons_com/Documents/BC Dev/Reports/PROD/Store Statistics/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT-DEV\Documents\BC-Projects\Store Statistics\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{13525EBA-74AF-4DEE-8E74-3DBBBC87BD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2964F2F7-1FA7-4C00-AAD0-1EAF1DD2BC86}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279D1EDE-6912-4976-91ED-0C7CCF05370A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="5" r:id="rId1"/>
@@ -20,9 +20,9 @@
     <sheet name="CaptionData" sheetId="3" state="hidden" r:id="rId5"/>
     <sheet name="Aggregated Metadata" sheetId="4" state="hidden" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <pivotCaches>
-    <pivotCache cacheId="22" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -265,10 +265,10 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Toatl Quantity</t>
-  </si>
-  <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Total Quantity</t>
   </si>
 </sst>
 </file>
@@ -339,11 +339,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -609,49 +609,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -735,49 +693,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -836,7 +752,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Toatl Quantity</c:v>
+                  <c:v>Total Quantity</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1914,7 +1830,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D8313C19-0EA8-4D27-88AE-64AE9A6F09B5}" name="PivotTable4" cacheId="22" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D8313C19-0EA8-4D27-88AE-64AE9A6F09B5}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
   <location ref="A4:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="23">
     <pivotField numFmtId="14" showAll="0"/>
@@ -1992,7 +1908,7 @@
     <pageField fld="2" hier="-1"/>
   </pageFields>
   <dataFields count="2">
-    <dataField name="Toatl Quantity" fld="10" baseField="0" baseItem="0"/>
+    <dataField name="Total Quantity" fld="10" baseField="18" baseItem="0"/>
     <dataField name="Total Cost" fld="11" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="12">
@@ -2515,15 +2431,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB6C94B0-627E-462A-B7AA-09DF1EE20EE7}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2536,7 +2452,7 @@
       <c r="A2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>0</v>
       </c>
     </row>
@@ -2545,29 +2461,29 @@
         <v>72</v>
       </c>
       <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" t="s">
         <v>74</v>
-      </c>
-      <c r="C4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="10">
         <v>0</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="8">
+      <c r="B6" s="10">
         <v>0</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2575,10 +2491,10 @@
       <c r="A7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="10">
         <v>0</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="10">
         <v>0</v>
       </c>
     </row>
@@ -2591,7 +2507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F361352-F8F4-49D7-B40B-1C9B2675306D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -2605,13 +2521,35 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:W2"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">

</xml_diff>